<commit_message>
first running version for single 10be nuclide
</commit_message>
<xml_diff>
--- a/Test_Input_Single_Be.xlsx
+++ b/Test_Input_Single_Be.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20380"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{117D24DA-DB13-4147-9444-1E505F5DB803}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E37FB750-D299-47C8-B675-731F2D0E80FE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="57">
   <si>
     <t>Sample</t>
   </si>
@@ -184,6 +184,9 @@
   </si>
   <si>
     <t>CDF</t>
+  </si>
+  <si>
+    <t>CDF_err</t>
   </si>
 </sst>
 </file>
@@ -951,38 +954,41 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B805AF-634F-468E-AD2E-541576FB2895}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>34</v>
       </c>
@@ -990,16 +996,19 @@
         <v>0.5</v>
       </c>
       <c r="C2" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="D2" s="9">
         <v>200</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="E2" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="F2" s="9" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
       <c r="B5" t="s">
         <v>48</v>

</xml_diff>

<commit_message>
just some step-size tuning in pairedCRN_MCMC
</commit_message>
<xml_diff>
--- a/Test_Input_Single_Be.xlsx
+++ b/Test_Input_Single_Be.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20380"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{127DBAA9-97BE-4BD5-8ED7-7FC5BE0C6880}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EA1539F-593E-41DA-B7A0-2650563C669C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="10Be Cronus" sheetId="3" r:id="rId1"/>
@@ -207,7 +207,7 @@
     <t>st</t>
   </si>
   <si>
-    <t>requires either bedrock or soil composition OR CDF</t>
+    <t>requires either bedrock or soil composition</t>
   </si>
 </sst>
 </file>
@@ -658,7 +658,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AI7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
@@ -987,8 +987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B805AF-634F-468E-AD2E-541576FB2895}">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
small changes towards using 10be without composition
</commit_message>
<xml_diff>
--- a/Test_Input_Single_Be.xlsx
+++ b/Test_Input_Single_Be.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20380"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EA1539F-593E-41DA-B7A0-2650563C669C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFCF4CEA-0CC8-4DAE-9B2F-BAFEEF2BF48C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -207,7 +207,7 @@
     <t>st</t>
   </si>
   <si>
-    <t>requires either bedrock or soil composition</t>
+    <t>optional: If you want to compute the regolith composition, enter a bedrock composition and vice versa</t>
   </si>
 </sst>
 </file>
@@ -302,7 +302,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -318,6 +318,7 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -988,7 +989,7 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1064,10 +1065,10 @@
       <c r="J2" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="K2" s="9">
+      <c r="K2" s="15">
         <v>50</v>
       </c>
-      <c r="L2" s="9">
+      <c r="L2" s="15">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
runing version with 10be missing compositional data
</commit_message>
<xml_diff>
--- a/Test_Input_Single_Be.xlsx
+++ b/Test_Input_Single_Be.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20380"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFCF4CEA-0CC8-4DAE-9B2F-BAFEEF2BF48C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3032C3C9-F202-4835-BDED-7F42129E0811}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -989,7 +989,7 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>